<commit_message>
Finished updating experimental data using new calibration curve, added master plot to do multisalinity plots
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaGlass_May11_2017/RaGlass_May11_2017.xlsx
+++ b/Sorption Experiments/RaGlass_May11_2017/RaGlass_May11_2017.xlsx
@@ -880,11 +880,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="221536544"/>
-        <c:axId val="221537328"/>
+        <c:axId val="213220352"/>
+        <c:axId val="213218784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="221536544"/>
+        <c:axId val="213220352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,12 +912,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221537328"/>
+        <c:crossAx val="213218784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="221537328"/>
+        <c:axId val="213218784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221536544"/>
+        <c:crossAx val="213220352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1180,11 +1180,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="221535760"/>
-        <c:axId val="221540464"/>
+        <c:axId val="213219960"/>
+        <c:axId val="213217216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="221535760"/>
+        <c:axId val="213219960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1212,12 +1212,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221540464"/>
+        <c:crossAx val="213217216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="221540464"/>
+        <c:axId val="213217216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,7 +1245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221535760"/>
+        <c:crossAx val="213219960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10288,7 +10288,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B2" sqref="B2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>